<commit_message>
Updated Design Interior + Surface
</commit_message>
<xml_diff>
--- a/BWB_Design_Interior/BWB_IO.xlsx
+++ b/BWB_Design_Interior/BWB_IO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\General Storage\TU Delft\MSc FPP\AE4204 KBE\BWB_Design_BETA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\General Storage\TU Delft\MSc FPP\AE4204 KBE\BWB_Design_Interior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2538107-A2AB-429B-998C-E7A1149EB490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762761CC-4F37-4B44-8D18-8082960EC75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CF6C8C78-A8A8-49BC-83DD-C17593CC9032}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CF6C8C78-A8A8-49BC-83DD-C17593CC9032}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Output_BWB" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
-  <si>
-    <t>Range</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>MTOW</t>
   </si>
@@ -82,9 +80,6 @@
   </si>
   <si>
     <t>OEW</t>
-  </si>
-  <si>
-    <t>NM</t>
   </si>
   <si>
     <t>m</t>
@@ -233,18 +228,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,33 +562,33 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
       <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
       </c>
       <c r="H1">
         <v>4554337</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2">
         <v>1234567</v>
@@ -614,7 +608,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,317 +631,306 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="4"/>
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="E1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>30</v>
+      <c r="A3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B3">
         <v>0.97</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>200</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>170600</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N3">
-        <v>52.4</v>
+        <v>60</v>
       </c>
       <c r="O3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="Q3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R3">
         <v>0.20499999999999999</v>
       </c>
       <c r="S3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>31</v>
+      <c r="A4" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B4">
         <v>0.98499999999999999</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4">
         <v>65000</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N4">
         <v>478</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R4">
         <v>13100</v>
       </c>
       <c r="S4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>32</v>
+      <c r="A5" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B5">
         <v>6000</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>3000</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J5">
         <v>15000</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>5.87</v>
       </c>
       <c r="O5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R5">
         <v>250</v>
       </c>
       <c r="S5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>33</v>
+      <c r="A6" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J6">
         <v>30000</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N6">
         <v>16</v>
       </c>
       <c r="O6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q6" t="s">
+        <v>43</v>
+      </c>
+      <c r="R6" s="4">
+        <v>1.8639000000000001E-4</v>
+      </c>
+      <c r="S6" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="6">
-        <v>1.8639000000000001E-4</v>
-      </c>
-      <c r="S6" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>32</v>
+      <c r="A7" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B7">
         <v>1000</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J7">
         <v>2800</v>
       </c>
       <c r="K7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q7" t="s">
-        <v>46</v>
-      </c>
-      <c r="R7" s="6">
+        <v>44</v>
+      </c>
+      <c r="R7" s="4">
         <v>1.8639000000000001E-4</v>
       </c>
       <c r="S7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>33</v>
+      <c r="A8" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B8">
         <v>0.5</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J8">
         <v>0.33</v>
       </c>
       <c r="K8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>34</v>
+      <c r="A9" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B9">
         <v>0.995</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J9">
         <v>0.6</v>
       </c>
       <c r="K9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>